<commit_message>
Adição de referência do Dicionário
</commit_message>
<xml_diff>
--- a/Artefato 2.4 - Caso de Uso - Dicionário de dados.xlsx
+++ b/Artefato 2.4 - Caso de Uso - Dicionário de dados.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade\3_Semestre\Análise e Modelagem de Sistemas\Exercicio_Prova\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willians.Pavelski\Downloads\Prova_Takuno-master\Prova_Takuno-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11CB3EE2-30A9-49A4-8294-8FD0EEEDE5E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1500" windowWidth="21705" windowHeight="12345" xr2:uid="{6DFCE9A2-72EA-4868-A49D-6F632B397B4E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Dicionário de Dados</t>
   </si>
@@ -84,9 +83,6 @@
     <t>Texto</t>
   </si>
   <si>
-    <t>Lista</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -106,12 +102,21 @@
   </si>
   <si>
     <t>NSA = Não se aplica</t>
+  </si>
+  <si>
+    <t>DC-01</t>
+  </si>
+  <si>
+    <t>DC-02</t>
+  </si>
+  <si>
+    <t>DC-03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,16 +478,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F778F81-4FD7-46D6-992D-C237AF264773}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="10" width="8.140625" customWidth="1"/>
@@ -535,8 +540,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -551,24 +556,24 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
       <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -577,62 +582,62 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>26</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>